<commit_message>
Passagem da página upload.html para dentro de index.html e sua melhoria na apresentação. Retirada na coluna id da planilha.
</commit_message>
<xml_diff>
--- a/teste.xlsx
+++ b/teste.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20389"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD7D82F-9988-4E42-8F86-A6FFBCF490FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC73E481-6A6C-405C-97F5-E252AAA281E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3090" yWindow="825" windowWidth="16410" windowHeight="9840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados" sheetId="2" r:id="rId1"/>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Nome</t>
   </si>
@@ -34,13 +31,13 @@
     <t>Sandro Boschetti</t>
   </si>
   <si>
-    <t>+553198334923</t>
-  </si>
-  <si>
-    <t>+5531996449238</t>
-  </si>
-  <si>
     <t>Madalena Oliveira</t>
+  </si>
+  <si>
+    <t>+553196449238</t>
+  </si>
+  <si>
+    <t>+553183349238</t>
   </si>
 </sst>
 </file>
@@ -375,49 +372,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F13A28A-6C33-4084-874F-430F1A665A61}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Conserto do problema de se não conseguir carregar novamente o arquivo com o mesmo nome, mesmo que tenha conteúdo diferente.
</commit_message>
<xml_diff>
--- a/teste.xlsx
+++ b/teste.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20389"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC73E481-6A6C-405C-97F5-E252AAA281E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E11DD9-8286-47DD-B4B8-DA9F88FDCDDF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3090" yWindow="825" windowWidth="16410" windowHeight="9840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -372,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F13A28A-6C33-4084-874F-430F1A665A61}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A4" sqref="A4:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -408,6 +408,54 @@
         <v>4</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="3"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Ajuste para o código não ler linhas com células vazias.
</commit_message>
<xml_diff>
--- a/teste.xlsx
+++ b/teste.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20389"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E11DD9-8286-47DD-B4B8-DA9F88FDCDDF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{436B0BED-594A-42AC-B64C-493A3348B365}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3090" yWindow="825" windowWidth="16410" windowHeight="9840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -372,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F13A28A-6C33-4084-874F-430F1A665A61}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B15"/>
+      <selection activeCell="A4" sqref="A4:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,6 +456,18 @@
       <c r="A15" s="1"/>
       <c r="B15" s="3"/>
     </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>